<commit_message>
Updated Deadline in School Registration Form
</commit_message>
<xml_diff>
--- a/assets/documents/BIPHMUN School Registration Form.xlsx
+++ b/assets/documents/BIPHMUN School Registration Form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\0 School\2025~2026\Model UN\Club\biphmun-related files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIPHMUN-Web\BIPHMUN-Web\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40C0BB1-BF45-4858-BEB0-02A8AB819137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C500AE-F17F-44E6-BAFC-049B5C844F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Withdrawal Deadline:</t>
   </si>
   <si>
-    <t>Feb 22nd, 2026</t>
-  </si>
-  <si>
     <t>Registration Info Section</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>UNEP</t>
+  </si>
+  <si>
+    <t>Feb 29th, 2026</t>
   </si>
 </sst>
 </file>
@@ -353,56 +353,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -776,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64461E1E-304B-4B64-9021-937170A1C2BB}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="14.3"/>
@@ -798,24 +796,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="F1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="10"/>
+      <c r="F1" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="19"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="22" t="s">
-        <v>22</v>
+      <c r="G2" s="15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -829,10 +827,10 @@
     </row>
     <row r="5" spans="1:9">
       <c r="F5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -840,171 +838,170 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="25.85" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="F9" s="24" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="F9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="F11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.3" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" ht="14.3" customHeight="1">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="G12" s="25"/>
-    </row>
-    <row r="13" spans="1:9" ht="14.3" customHeight="1">
-      <c r="A13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="13"/>
       <c r="F13" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="12"/>
       <c r="F14" s="23"/>
       <c r="G14" s="23"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="12"/>
       <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
         <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="s">
         <v>34</v>
       </c>
-      <c r="G16" t="s">
+    </row>
+    <row r="17" spans="1:14" ht="14.3" customHeight="1">
+      <c r="B17" s="5"/>
+      <c r="F17" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" ht="14.3" customHeight="1">
-      <c r="B17" s="8"/>
-      <c r="F17" t="s">
+      <c r="G17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="21" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="18" spans="1:14" ht="14.3" customHeight="1">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="5" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="5"/>
+      <c r="M18" s="20"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="K19" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L19" s="4" t="s">
+      <c r="L19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="4" t="s">
-        <v>40</v>
+      <c r="N19" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1031,7 +1028,7 @@
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="C24" s="16"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:14">
       <c r="A25">
@@ -1059,200 +1056,71 @@
       </c>
     </row>
     <row r="35" spans="1:13" ht="16.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="18"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="7"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="M35" s="12"/>
-    </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="13"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="13"/>
+      <c r="G36" s="8"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
+      <c r="F37" s="4"/>
     </row>
     <row r="38" spans="1:13">
       <c r="A38">
         <v>2</v>
       </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
-      <c r="J38" s="12"/>
-      <c r="K38" s="12"/>
     </row>
     <row r="39" spans="1:13">
       <c r="A39">
         <v>3</v>
       </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
-      <c r="K39" s="12"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:13">
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="1:13">
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
-    </row>
-    <row r="43" spans="1:13">
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="H46" s="12"/>
-      <c r="I46" s="12"/>
-      <c r="J46" s="12"/>
-      <c r="K46" s="12"/>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="H48" s="12"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12"/>
-    </row>
-    <row r="49" spans="8:11">
-      <c r="H49" s="12"/>
-      <c r="I49" s="12"/>
-      <c r="J49" s="12"/>
-      <c r="K49" s="12"/>
-    </row>
-    <row r="50" spans="8:11">
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="K50" s="12"/>
-    </row>
-    <row r="51" spans="8:11">
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
-      <c r="J51" s="12"/>
-      <c r="K51" s="12"/>
-    </row>
-    <row r="52" spans="8:11">
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12"/>
-      <c r="K52" s="12"/>
-    </row>
-    <row r="53" spans="8:11">
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12"/>
-      <c r="K53" s="12"/>
-    </row>
-    <row r="54" spans="8:11">
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-    </row>
-    <row r="55" spans="8:11">
-      <c r="H55" s="12"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-    </row>
-    <row r="56" spans="8:11">
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-    </row>
-    <row r="57" spans="8:11">
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F13:G14"/>
     <mergeCell ref="A10:D11"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H18:K18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F13:G14"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:K34" xr:uid="{DD9FE948-F847-4008-839A-CDF18DDC26E4}">

</xml_diff>

<commit_message>
Modified School Registration Form
</commit_message>
<xml_diff>
--- a/assets/documents/BIPHMUN School Registration Form.xlsx
+++ b/assets/documents/BIPHMUN School Registration Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIPHMUN-Web\BIPHMUN-Web\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C500AE-F17F-44E6-BAFC-049B5C844F26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C9F1B4-126E-4674-B4F6-939870855070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>BIPHMUN School Registration Form</t>
   </si>
@@ -135,12 +135,6 @@
     <t>账号：</t>
   </si>
   <si>
-    <t>39297203003808500</t>
-  </si>
-  <si>
-    <t>Registration is only confirmed after payment has been received. Please add a note for the payment.</t>
-  </si>
-  <si>
     <t>Chair Names</t>
   </si>
   <si>
@@ -153,9 +147,6 @@
     <t>Chair application form:</t>
   </si>
   <si>
-    <t>Note: Please fill in the following form for chair applications. The Chairs section below is only for accommodations and other info</t>
-  </si>
-  <si>
     <t>Abbreviated School Name:</t>
   </si>
   <si>
@@ -174,7 +165,46 @@
     <t>UNEP</t>
   </si>
   <si>
-    <t>Feb 29th, 2026</t>
+    <r>
+      <t xml:space="preserve">Please add a note in the transfer stating </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF0A4D7F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>your school name, number of delegates and number of chairs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to help us validate your registration.</t>
+    </r>
+  </si>
+  <si>
+    <t>Note: Please fill in the following form for chair applications. The Chairs section in the table below is only for accommodations and other information</t>
+  </si>
+  <si>
+    <t>Registration is only confirmed after payment has been received. Please add a note for the payment as mentioned above</t>
+  </si>
+  <si>
+    <t>0039297203003808500</t>
+  </si>
+  <si>
+    <t>Payment is only accepted via Bank Transfer</t>
+  </si>
+  <si>
+    <t>Feb 28th, 2026</t>
   </si>
 </sst>
 </file>
@@ -248,13 +278,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -265,6 +288,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0A4D7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,29 +409,29 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -411,8 +442,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0A4D7F"/>
       <color rgb="FFD8EDFC"/>
-      <color rgb="FF0A4D7F"/>
       <color rgb="FFD9DAFF"/>
       <color rgb="FFF2F2F2"/>
     </mruColors>
@@ -777,7 +808,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="14.3"/>
@@ -795,120 +826,145 @@
     <col min="13" max="13" width="26.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="F1" s="19" t="s">
+    <row r="1" spans="1:10" ht="14.3" customHeight="1">
+      <c r="F1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="19"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="G1" s="23"/>
+      <c r="I1" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="F2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>51</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" ht="14.3" customHeight="1">
       <c r="F3" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="F5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="F6" t="s">
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>51</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="F7" t="s">
         <v>23</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="25.85" customHeight="1">
-      <c r="A9" s="21" t="s">
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+    </row>
+    <row r="9" spans="1:10" ht="25.85" customHeight="1">
+      <c r="A9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="F9" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="F11" t="s">
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="F9" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.3" customHeight="1">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.3" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="G12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" ht="14.3" customHeight="1">
+      <c r="F12" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:10" ht="14.3" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="F13" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="23"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="F13" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -920,7 +976,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="F16" t="s">
         <v>33</v>
       </c>
@@ -934,31 +990,31 @@
         <v>35</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.3" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="20" t="s">
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="20"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="3" t="s">
@@ -983,16 +1039,16 @@
         <v>5</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>7</v>
@@ -1001,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1059,14 +1115,14 @@
       <c r="A35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18" t="s">
+      <c r="B35" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
@@ -1087,7 +1143,7 @@
         <v>29</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G36" s="8"/>
       <c r="L36" s="9"/>
@@ -1110,17 +1166,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="I1:J8"/>
+    <mergeCell ref="F13:H14"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="B18:G18"/>
     <mergeCell ref="A9:D9"/>
     <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F13:G14"/>
     <mergeCell ref="A10:D11"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H18:K18"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:K34" xr:uid="{DD9FE948-F847-4008-839A-CDF18DDC26E4}">
@@ -1133,7 +1191,7 @@
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" xr:uid="{88494F8C-0788-4171-AD89-D587CB46D1AA}"/>
     <hyperlink ref="G7" r:id="rId2" xr:uid="{D007BBFC-8084-4F10-8C19-A476107509D5}"/>
-    <hyperlink ref="G11" r:id="rId3" display="https://forms.office.com/r/CjfTJMapVf" xr:uid="{FDC2C7ED-DA5F-4443-AC03-422FFA7C1332}"/>
+    <hyperlink ref="G10" r:id="rId3" display="https://forms.office.com/r/CjfTJMapVf" xr:uid="{FDC2C7ED-DA5F-4443-AC03-422FFA7C1332}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>

<commit_message>
Updated School Registration Form
</commit_message>
<xml_diff>
--- a/assets/documents/BIPHMUN School Registration Form.xlsx
+++ b/assets/documents/BIPHMUN School Registration Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIPHMUN-Web\BIPHMUN-Web\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C9F1B4-126E-4674-B4F6-939870855070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71FB79F-A9E0-4C7C-8239-D8EA2D8DB75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
+    <workbookView xWindow="3423" yWindow="3423" windowWidth="17810" windowHeight="10325" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
   </bookViews>
   <sheets>
     <sheet name="School Registration Form" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Abbreviated School Name:</t>
-  </si>
-  <si>
-    <t>Thank you for your interest in BIPHMUN 2026. Please email the completed form by Feb 22nd to mun-biph@basischina.com. Additional Info would be sent via email.</t>
   </si>
   <si>
     <t>SC</t>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Feb 28th, 2026</t>
+  </si>
+  <si>
+    <t>Thank you for your interest in BIPHMUN 2026. Please email the completed form by Feb 28th to mun-biph@basischina.com. Additional Info would be sent via email.</t>
   </si>
 </sst>
 </file>
@@ -410,28 +410,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,7 +808,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="14.3"/>
@@ -827,24 +827,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.3" customHeight="1">
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="I1" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="21"/>
+      <c r="G1" s="17"/>
+      <c r="I1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10">
       <c r="F2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+        <v>50</v>
+      </c>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
     </row>
     <row r="3" spans="1:10" ht="14.3" customHeight="1">
       <c r="F3" t="s">
@@ -853,8 +853,8 @@
       <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
     </row>
     <row r="4" spans="1:10">
       <c r="F4" s="1" t="s">
@@ -863,8 +863,8 @@
       <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10">
       <c r="F5" s="1" t="s">
@@ -873,18 +873,18 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10">
       <c r="F6" t="s">
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+        <v>50</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10">
       <c r="F7" t="s">
@@ -893,34 +893,34 @@
       <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" ht="25.85" customHeight="1">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="F9" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="F9" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="A10" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
       <c r="F10" t="s">
         <v>39</v>
       </c>
@@ -929,40 +929,40 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
     </row>
     <row r="12" spans="1:10" ht="14.3" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="F12" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="G12" s="22"/>
+      <c r="F12" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:10" ht="14.3" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="F13" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="F13" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
@@ -990,31 +990,31 @@
         <v>35</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.3" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="16" t="s">
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="16"/>
+      <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="3" t="s">
@@ -1039,16 +1039,16 @@
         <v>5</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>7</v>
@@ -1115,14 +1115,14 @@
       <c r="A35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17" t="s">
+      <c r="C35" s="16"/>
+      <c r="D35" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="17"/>
+      <c r="E35" s="16"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
@@ -1167,6 +1167,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A10:D11"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="F1:G1"/>
@@ -1174,11 +1179,6 @@
     <mergeCell ref="I1:J8"/>
     <mergeCell ref="F13:H14"/>
     <mergeCell ref="F12:G12"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="A10:D11"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:K34" xr:uid="{DD9FE948-F847-4008-839A-CDF18DDC26E4}">

</xml_diff>

<commit_message>
updated form for account info
</commit_message>
<xml_diff>
--- a/assets/documents/BIPHMUN School Registration Form.xlsx
+++ b/assets/documents/BIPHMUN School Registration Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BIPHMUN-Web\BIPHMUN-Web\assets\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71FB79F-A9E0-4C7C-8239-D8EA2D8DB75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DA2E95-9CF9-441A-B621-E514306D9A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3423" yWindow="3423" windowWidth="17810" windowHeight="10325" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889" xr2:uid="{2C198DE5-D1A7-4931-8CCC-D872BBFC0042}"/>
   </bookViews>
   <sheets>
     <sheet name="School Registration Form" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>开户行：</t>
   </si>
   <si>
-    <t>上海银行深圳君汇支行</t>
-  </si>
-  <si>
     <t>账号：</t>
   </si>
   <si>
@@ -160,6 +157,27 @@
   </si>
   <si>
     <t>UNEP</t>
+  </si>
+  <si>
+    <t>Note: Please fill in the following form for chair applications. The Chairs section in the table below is only for accommodations and other information</t>
+  </si>
+  <si>
+    <t>Registration is only confirmed after payment has been received. Please add a note for the payment as mentioned above</t>
+  </si>
+  <si>
+    <t>Payment is only accepted via Bank Transfer</t>
+  </si>
+  <si>
+    <t>Feb 28th, 2026</t>
+  </si>
+  <si>
+    <t>Thank you for your interest in BIPHMUN 2026. Please email the completed form by Feb 28th to mun-biph@basischina.com. Additional Info would be sent via email.</t>
+  </si>
+  <si>
+    <t>交通银行深圳华侨城支行</t>
+  </si>
+  <si>
+    <t>443066333013005129594</t>
   </si>
   <si>
     <r>
@@ -174,7 +192,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>your school name, number of delegates and number of chairs</t>
+      <t>your school name + number of delegates + number of chairs + "MUN"</t>
     </r>
     <r>
       <rPr>
@@ -187,24 +205,6 @@
       </rPr>
       <t xml:space="preserve"> to help us validate your registration.</t>
     </r>
-  </si>
-  <si>
-    <t>Note: Please fill in the following form for chair applications. The Chairs section in the table below is only for accommodations and other information</t>
-  </si>
-  <si>
-    <t>Registration is only confirmed after payment has been received. Please add a note for the payment as mentioned above</t>
-  </si>
-  <si>
-    <t>0039297203003808500</t>
-  </si>
-  <si>
-    <t>Payment is only accepted via Bank Transfer</t>
-  </si>
-  <si>
-    <t>Feb 28th, 2026</t>
-  </si>
-  <si>
-    <t>Thank you for your interest in BIPHMUN 2026. Please email the completed form by Feb 28th to mun-biph@basischina.com. Additional Info would be sent via email.</t>
   </si>
 </sst>
 </file>
@@ -410,28 +410,28 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -808,7 +808,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="14.3"/>
@@ -827,24 +827,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.3" customHeight="1">
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="I1" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="18"/>
+      <c r="G1" s="21"/>
+      <c r="I1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10">
       <c r="F2" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
     </row>
     <row r="3" spans="1:10" ht="14.3" customHeight="1">
       <c r="F3" t="s">
@@ -853,8 +853,8 @@
       <c r="G3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
     </row>
     <row r="4" spans="1:10">
       <c r="F4" s="1" t="s">
@@ -863,8 +863,8 @@
       <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10">
       <c r="F5" s="1" t="s">
@@ -873,18 +873,18 @@
       <c r="G5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
     </row>
     <row r="6" spans="1:10">
       <c r="F6" t="s">
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
     </row>
     <row r="7" spans="1:10">
       <c r="F7" t="s">
@@ -893,76 +893,76 @@
       <c r="G7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
     </row>
     <row r="9" spans="1:10" ht="25.85" customHeight="1">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="F9" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="F9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:10" ht="14.3" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="11"/>
-      <c r="F12" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="20"/>
+      <c r="F12" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="23"/>
     </row>
     <row r="13" spans="1:10" ht="14.3" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="F13" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
+      <c r="F13" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="12"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
@@ -981,40 +981,40 @@
         <v>33</v>
       </c>
       <c r="G16" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="14.3" customHeight="1">
       <c r="B17" s="5"/>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="14.3" customHeight="1">
       <c r="A18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16" t="s">
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="16"/>
-      <c r="L18" s="21" t="s">
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M18" s="21"/>
+      <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:14">
       <c r="A19" s="3" t="s">
@@ -1039,16 +1039,16 @@
         <v>5</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="K19" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>7</v>
@@ -1057,7 +1057,7 @@
         <v>9</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1115,14 +1115,14 @@
       <c r="A35" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16" t="s">
+      <c r="B35" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="16"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
     </row>
@@ -1143,7 +1143,7 @@
         <v>29</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G36" s="8"/>
       <c r="L36" s="9"/>
@@ -1167,11 +1167,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="A10:D11"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="F1:G1"/>
@@ -1179,8 +1174,13 @@
     <mergeCell ref="I1:J8"/>
     <mergeCell ref="F13:H14"/>
     <mergeCell ref="F12:G12"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="A10:D11"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:K34" xr:uid="{DD9FE948-F847-4008-839A-CDF18DDC26E4}">
       <formula1>"1,2,3,4"</formula1>
     </dataValidation>

</xml_diff>